<commit_message>
Fixed chart caption error from incorrect formula reference.
</commit_message>
<xml_diff>
--- a/analysis/The cost of reaching herd immunity.xlsx
+++ b/analysis/The cost of reaching herd immunity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/projects/BeachAnalytics/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51B3EE8-CBA1-EC42-A4BC-4B72022E6DA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6716C193-3C67-7242-8643-F70D272BDE50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{B3DEE8B6-B165-0444-A2CF-347D664BBB9D}"/>
   </bookViews>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="19">
   <si>
     <t>area</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>infections</t>
+  </si>
+  <si>
+    <t>https://beachanalytics.info/2020/05/23/estimating-the-cost-of-reaching-herd-immunity.html</t>
   </si>
 </sst>
 </file>
@@ -16131,7 +16134,7 @@
               <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
               <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
             </a:rPr>
-            <a:t>There have been about 96 thousand deaths out of about 1.9 million infections so far.</a:t>
+            <a:t>There have been about 96 thousand deaths out of about 13.5 million infections so far.</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1300">
             <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
@@ -18345,7 +18348,7 @@
               <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
-            <a:t>There have been about 2,200 deaths out of about 139,000 infections so far.</a:t>
+            <a:t>There have been about 2,200 deaths out of about 279,000 infections so far.</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1300">
             <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
@@ -20601,7 +20604,7 @@
               <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
-            <a:t>There have been about 600 deaths out of about 21,000 infections so far.</a:t>
+            <a:t>There have been about 600 deaths out of about 66,000 infections so far.</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1300">
             <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
@@ -22897,7 +22900,7 @@
               <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
-            <a:t>There have been about 300 deaths out of about 18,000 infections so far.</a:t>
+            <a:t>There have been about 300 deaths out of about 26,000 infections so far.</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1300">
             <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
@@ -25395,7 +25398,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -25673,8 +25676,8 @@
       <c r="H15" s="17"/>
       <c r="I15" s="18"/>
       <c r="K15" s="2" t="str">
-        <f>"There have been about " &amp; TEXT(ROUND(K5/1000, 3),"#") &amp; " thousand deaths out of about " &amp; TEXT(ROUND(K9/1000000, 3),"#.#") &amp; " million infections so far."</f>
-        <v>There have been about 96 thousand deaths out of about 1.9 million infections so far.</v>
+        <f>"There have been about " &amp; TEXT(ROUND(K5/1000, 3),"#") &amp; " thousand deaths out of about " &amp; TEXT(ROUND(L5/1000000, 3),"#.#") &amp; " million infections so far."</f>
+        <v>There have been about 96 thousand deaths out of about 13.5 million infections so far.</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -25717,6 +25720,9 @@
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
       <c r="I18" s="18"/>
+      <c r="K18" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="16"/>
@@ -25946,8 +25952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DF63B9E-9E91-2746-B9A3-D8CD57A4E626}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -26225,8 +26231,8 @@
       <c r="H15" s="17"/>
       <c r="I15" s="18"/>
       <c r="K15" s="2" t="str">
-        <f>"There have been about " &amp; TEXT(ROUND(K5, -2),"#,#") &amp; " deaths out of about " &amp; TEXT(ROUND(K9, -3),"#,#") &amp; " infections so far."</f>
-        <v>There have been about 2,200 deaths out of about 139,000 infections so far.</v>
+        <f>"There have been about " &amp; TEXT(ROUND(K5, -2),"#,#") &amp; " deaths out of about " &amp; TEXT(ROUND(L5, -3),"#,#") &amp; " infections so far."</f>
+        <v>There have been about 2,200 deaths out of about 279,000 infections so far.</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -26498,8 +26504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB22BA92-0C2C-B545-8B1C-D6A67FE7E424}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -26777,8 +26783,8 @@
       <c r="H15" s="17"/>
       <c r="I15" s="18"/>
       <c r="K15" s="2" t="str">
-        <f>"There have been about " &amp; TEXT(ROUND(K5, -2),"#,#") &amp; " deaths out of about " &amp; TEXT(ROUND(K9, -3),"#,#") &amp; " infections so far."</f>
-        <v>There have been about 600 deaths out of about 21,000 infections so far.</v>
+        <f>"There have been about " &amp; TEXT(ROUND(K5, -2),"#,#") &amp; " deaths out of about " &amp; TEXT(ROUND(L5, -3),"#,#") &amp; " infections so far."</f>
+        <v>There have been about 600 deaths out of about 66,000 infections so far.</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -27050,8 +27056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A7D4B9D-CC0D-3D4F-95FE-FAB091587049}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -27329,8 +27335,8 @@
       <c r="H15" s="17"/>
       <c r="I15" s="18"/>
       <c r="K15" s="2" t="str">
-        <f>"There have been about " &amp; TEXT(ROUND(K5, -2),"#,#") &amp; " deaths out of about " &amp; TEXT(ROUND(K9, -3),"#,#") &amp; " infections so far."</f>
-        <v>There have been about 300 deaths out of about 18,000 infections so far.</v>
+        <f>"There have been about " &amp; TEXT(ROUND(K5, -2),"#,#") &amp; " deaths out of about " &amp; TEXT(ROUND(L5, -3),"#,#") &amp; " infections so far."</f>
+        <v>There have been about 300 deaths out of about 26,000 infections so far.</v>
       </c>
     </row>
     <row r="16" spans="1:16">

</xml_diff>

<commit_message>
Fixed URL in the cost-of-herd-immunity charts.
Many thanks to Calleigh Alice for the QA on that.
</commit_message>
<xml_diff>
--- a/analysis/The cost of reaching herd immunity.xlsx
+++ b/analysis/The cost of reaching herd immunity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/projects/BeachAnalytics/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6716C193-3C67-7242-8643-F70D272BDE50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036313A7-020D-7944-8301-5AAEB24352A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{B3DEE8B6-B165-0444-A2CF-347D664BBB9D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B3DEE8B6-B165-0444-A2CF-347D664BBB9D}"/>
   </bookViews>
   <sheets>
     <sheet name="US" sheetId="1" r:id="rId1"/>
@@ -15894,13 +15894,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>77556</xdr:rowOff>
+      <xdr:rowOff>95073</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>602153</xdr:colOff>
+      <xdr:colOff>602152</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>145854</xdr:rowOff>
+      <xdr:rowOff>144517</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -15915,8 +15915,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="0" y="7174615"/>
-          <a:ext cx="5554086" cy="271071"/>
+          <a:off x="0" y="7145763"/>
+          <a:ext cx="5568290" cy="250892"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16011,21 +16011,15 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1">
+            <a:rPr lang="en-US" sz="1200" b="0" i="0">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+              <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+              <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
             </a:rPr>
-            <a:t>Explanation and sources at https://BeachAnalytics/cost-of-herd-immunity</a:t>
+            <a:t>Explanation and sources at https://BeachAnalytics.info/cost-of-herd-immunity</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="1">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
-            <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -18107,13 +18101,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>77557</xdr:rowOff>
+      <xdr:rowOff>96608</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>602153</xdr:colOff>
+      <xdr:colOff>602152</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>150856</xdr:rowOff>
+      <xdr:rowOff>155576</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -18128,8 +18122,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="0" y="7199380"/>
-          <a:ext cx="5548838" cy="276780"/>
+          <a:off x="0" y="7208608"/>
+          <a:ext cx="5555152" cy="262168"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -18224,21 +18218,15 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1">
+            <a:rPr lang="en-US" sz="1200" b="0" i="0">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+              <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+              <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
             </a:rPr>
-            <a:t>Explanation and sources at https://BeachAnalytics/cost-of-herd-immunity</a:t>
+            <a:t>Explanation and sources at https://BeachAnalytics.info/cost-of-herd-immunity</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="1">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
-            <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -20363,13 +20351,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>77557</xdr:rowOff>
+      <xdr:rowOff>87301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>602154</xdr:colOff>
+      <xdr:colOff>602153</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>155575</xdr:rowOff>
+      <xdr:rowOff>146163</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -20384,8 +20372,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="0" y="7189557"/>
-          <a:ext cx="5555154" cy="281218"/>
+          <a:off x="0" y="7249321"/>
+          <a:ext cx="5552230" cy="263492"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -20480,21 +20468,15 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1">
+            <a:rPr lang="en-US" sz="1200" b="0" i="0">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+              <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+              <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
             </a:rPr>
-            <a:t>Explanation and sources at https://BeachAnalytics/cost-of-herd-immunity</a:t>
+            <a:t>Explanation and sources at https://BeachAnalytics.info/cost-of-herd-immunity</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="1">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
-            <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -22776,21 +22758,15 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1">
+            <a:rPr lang="en-US" sz="1200" b="0" i="0">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+              <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+              <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
             </a:rPr>
-            <a:t>Explanation and sources at https://BeachAnalytics/cost-of-herd-immunity</a:t>
+            <a:t>Explanation and sources at https://BeachAnalytics.info/cost-of-herd-immunity</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="1">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
-            <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -25397,8 +25373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F2722A-BA5A-8646-9F79-9A5DAC7DF673}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -25952,8 +25928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DF63B9E-9E91-2746-B9A3-D8CD57A4E626}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView topLeftCell="C27" zoomScale="297" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -26504,8 +26480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB22BA92-0C2C-B545-8B1C-D6A67FE7E424}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -27056,8 +27032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A7D4B9D-CC0D-3D4F-95FE-FAB091587049}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Copy tweaks and timestamp update for Outlook.
</commit_message>
<xml_diff>
--- a/analysis/The cost of reaching herd immunity.xlsx
+++ b/analysis/The cost of reaching herd immunity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/projects/BeachAnalytics/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036313A7-020D-7944-8301-5AAEB24352A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC30307-DAFC-7F44-B999-593D2ECA3640}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B3DEE8B6-B165-0444-A2CF-347D664BBB9D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{B3DEE8B6-B165-0444-A2CF-347D664BBB9D}"/>
   </bookViews>
   <sheets>
     <sheet name="US" sheetId="1" r:id="rId1"/>
@@ -19,57 +19,7 @@
     <sheet name="Broward" sheetId="6" r:id="rId4"/>
     <sheet name="data" sheetId="2" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">US!$K$11</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">US!$K$12</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">US!$L$4</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">US!$L$5</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">US!$K$11</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">US!$K$12</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">US!$K$4</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">US!$K$5</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">US!$L$4</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">US!$L$5</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">US!$K$11</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">US!$K$12</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">US!$K$4</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">US!$K$4</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">US!$K$5</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">US!$L$4</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">US!$L$5</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">US!$K$11</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">US!$K$12</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">US!$K$4</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">US!$K$5</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">US!$L$4</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">US!$L$5</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">US!$K$5</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">US!$K$11</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">US!$K$12</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">US!$K$4</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">US!$K$5</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">US!$L$4</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">US!$L$5</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">US!$K$11</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">US!$K$12</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">US!$K$4</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">US!$K$5</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">US!$L$4</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">US!$L$4</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">US!$L$5</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">US!$K$11</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">US!$K$12</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">US!$K$4</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">US!$K$5</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">US!$L$4</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">US!$L$5</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">US!$L$5</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">US!$K$11</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">US!$K$12</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">US!$K$4</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">US!$K$5</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -109,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="18">
   <si>
     <t>area</t>
   </si>
@@ -163,9 +113,6 @@
   </si>
   <si>
     <t>infections</t>
-  </si>
-  <si>
-    <t>https://beachanalytics.info/2020/05/23/estimating-the-cost-of-reaching-herd-immunity.html</t>
   </si>
 </sst>
 </file>
@@ -348,6 +295,183 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="94">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1451,6 +1575,42 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1461,7 +1621,20 @@
         <name val="Inconsolata"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1476,19 +1649,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1555,150 +1715,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1744,13 +1761,6 @@
         <name val="Inconsolata"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDEECF7"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1768,160 +1778,7 @@
         <name val="Inconsolata"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDEECF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDEECF7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <scheme val="none"/>
-      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1992,6 +1849,96 @@
         <name val="Inconsolata"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDEECF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDEECF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDEECF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -16128,6 +16075,7 @@
               <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
               <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>There have been about 96 thousand deaths out of about 13.5 million infections so far.</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1300">
@@ -16204,6 +16152,7 @@
               <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
               <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>About 81% of the population could be infected if the virus were to spread uncontrolled.</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1300">
@@ -16280,6 +16229,7 @@
               <a:latin typeface="Roboto Medium" panose="02000000000000000000" pitchFamily="2" charset="0"/>
               <a:ea typeface="Roboto Medium" panose="02000000000000000000" pitchFamily="2" charset="0"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>At the current fatality rate, reaching herd immunity could cost about 1.9 million lives.</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1300" b="0" i="0">
@@ -18336,6 +18286,7 @@
               <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>There have been about 2,200 deaths out of about 279,000 infections so far.</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1300">
@@ -18413,6 +18364,7 @@
               <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>About 81% of the population could be infected if the virus were to spread uncontrolled.</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1300">
@@ -18490,6 +18442,7 @@
               <a:ea typeface="Roboto Medium" panose="02000000000000000000" pitchFamily="2" charset="0"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>At the current fatality rate, reaching herd immunity could cost about 140,000 lives.</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1300" b="0" i="0">
@@ -20586,6 +20539,7 @@
               <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>There have been about 600 deaths out of about 66,000 infections so far.</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1300">
@@ -20663,6 +20617,7 @@
               <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>About 81% of the population could be infected if the virus were to spread uncontrolled.</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1300">
@@ -20740,6 +20695,7 @@
               <a:ea typeface="Roboto Medium" panose="02000000000000000000" pitchFamily="2" charset="0"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>At the current fatality rate, reaching herd immunity could cost about 20,000 lives.</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1300" b="0" i="0">
@@ -22876,6 +22832,7 @@
               <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>There have been about 300 deaths out of about 26,000 infections so far.</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1300">
@@ -22953,6 +22910,7 @@
               <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>About 81% of the population could be infected if the virus were to spread uncontrolled.</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1300">
@@ -23030,6 +22988,7 @@
               <a:ea typeface="Roboto Medium" panose="02000000000000000000" pitchFamily="2" charset="0"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>At the current fatality rate, reaching herd immunity could cost about 20,000 lives.</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1300" b="0" i="0">
@@ -24760,12 +24719,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{68937E22-76C4-CD45-A428-8FAD25BA84D8}" name="Table2" displayName="Table2" ref="K4:L5" totalsRowShown="0" headerRowDxfId="78" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{68937E22-76C4-CD45-A428-8FAD25BA84D8}" name="Table2" displayName="Table2" ref="K4:L5" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
   <tableColumns count="2">
-    <tableColumn id="3" xr3:uid="{E180202B-D5B3-D748-9987-31BA1F47523E}" name="deaths" dataDxfId="80">
+    <tableColumn id="3" xr3:uid="{E180202B-D5B3-D748-9987-31BA1F47523E}" name="deaths" dataDxfId="91">
       <calculatedColumnFormula>data!B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{7FDFD004-E1E7-2A47-9BBC-A4FDBC7E9D8B}" name="estimated number of infections" dataDxfId="82">
+    <tableColumn id="1" xr3:uid="{7FDFD004-E1E7-2A47-9BBC-A4FDBC7E9D8B}" name="estimated number of infections" dataDxfId="90">
       <calculatedColumnFormula>data!F2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -24774,15 +24733,15 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{11BF5025-29AD-BD45-B117-E670B85E6687}" name="Table617" displayName="Table617" ref="N8:P9" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{11BF5025-29AD-BD45-B117-E670B85E6687}" name="Table617" displayName="Table617" ref="N8:P9" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{BD3EB270-B4B0-C146-B4A0-D227CE94FB85}" name="deaths" dataDxfId="44">
+    <tableColumn id="1" xr3:uid="{BD3EB270-B4B0-C146-B4A0-D227CE94FB85}" name="deaths" dataDxfId="54">
       <calculatedColumnFormula>Table314[[#This Row],[projected deaths at 81% prevalence]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E08C978F-0670-114C-8F46-50CDC4F4FA6A}" name="infections" dataDxfId="43">
+    <tableColumn id="2" xr3:uid="{E08C978F-0670-114C-8F46-50CDC4F4FA6A}" name="infections" dataDxfId="53">
       <calculatedColumnFormula>Table314[[#This Row],[number of infections]]-Table314[[#This Row],[projected deaths at 81% prevalence]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BA1A334E-04F6-2D4A-A0BE-BAD26F3921D0}" name="population" dataDxfId="42">
+    <tableColumn id="3" xr3:uid="{BA1A334E-04F6-2D4A-A0BE-BAD26F3921D0}" name="population" dataDxfId="52">
       <calculatedColumnFormula array="1">Table415[population]-(O9+N9)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -24791,12 +24750,12 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{AEDA19CC-3088-4144-8B82-AEAB0F7CC8D0}" name="Table21318" displayName="Table21318" ref="K4:L5" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{AEDA19CC-3088-4144-8B82-AEAB0F7CC8D0}" name="Table21318" displayName="Table21318" ref="K4:L5" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <tableColumns count="2">
-    <tableColumn id="3" xr3:uid="{58614EA6-2D78-BD44-997F-C09426388E83}" name="deaths" dataDxfId="39">
+    <tableColumn id="3" xr3:uid="{58614EA6-2D78-BD44-997F-C09426388E83}" name="deaths" dataDxfId="49">
       <calculatedColumnFormula>data!B4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{829F51ED-B66A-5F47-AB0D-19EE23DBAA12}" name="estimated number of infections" dataDxfId="38">
+    <tableColumn id="1" xr3:uid="{829F51ED-B66A-5F47-AB0D-19EE23DBAA12}" name="estimated number of infections" dataDxfId="48">
       <calculatedColumnFormula>data!F4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -24805,12 +24764,12 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{C8073B54-F6EA-F741-839A-352408146B3D}" name="Table31419" displayName="Table31419" ref="K8:L9" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{C8073B54-F6EA-F741-839A-352408146B3D}" name="Table31419" displayName="Table31419" ref="K8:L9" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <tableColumns count="2">
-    <tableColumn id="3" xr3:uid="{BCC16318-4AC1-0240-B0DD-A288AD2F0632}" name="projected deaths at 81% prevalence" dataDxfId="35">
+    <tableColumn id="3" xr3:uid="{BCC16318-4AC1-0240-B0DD-A288AD2F0632}" name="projected deaths at 81% prevalence" dataDxfId="45">
       <calculatedColumnFormula>data!H4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{3870A287-BC3F-B346-98A2-2E45C07E4D19}" name="number of infections" dataDxfId="34">
+    <tableColumn id="1" xr3:uid="{3870A287-BC3F-B346-98A2-2E45C07E4D19}" name="number of infections" dataDxfId="44">
       <calculatedColumnFormula>data!G4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -24819,9 +24778,9 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{A034DC94-401E-6A42-A6CB-DD47F86E04FC}" name="Table41520" displayName="Table41520" ref="K11:K12" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{A034DC94-401E-6A42-A6CB-DD47F86E04FC}" name="Table41520" displayName="Table41520" ref="K11:K12" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{07122545-26F0-0640-8EA3-87D8D4439587}" name="population" dataDxfId="31">
+    <tableColumn id="1" xr3:uid="{07122545-26F0-0640-8EA3-87D8D4439587}" name="population" dataDxfId="41">
       <calculatedColumnFormula>data!C4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -24830,15 +24789,15 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{192F3784-6F3E-0B43-A70B-0A7BD18DB0B0}" name="Table51621" displayName="Table51621" ref="N4:P5" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{192F3784-6F3E-0B43-A70B-0A7BD18DB0B0}" name="Table51621" displayName="Table51621" ref="N4:P5" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A318F5C1-C985-2646-9EF6-A65AC959B1F8}" name="deaths" dataDxfId="28">
+    <tableColumn id="1" xr3:uid="{A318F5C1-C985-2646-9EF6-A65AC959B1F8}" name="deaths" dataDxfId="38">
       <calculatedColumnFormula>Table21318[[#This Row],[deaths]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{8AB70894-0C9F-854E-B008-9BC55264895C}" name="infections" dataDxfId="27">
+    <tableColumn id="2" xr3:uid="{8AB70894-0C9F-854E-B008-9BC55264895C}" name="infections" dataDxfId="37">
       <calculatedColumnFormula>Table21318[[#This Row],[estimated number of infections]]-N5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{3C6E783B-60EC-F249-9BBB-E5313DD53FB2}" name="population" dataDxfId="26">
+    <tableColumn id="3" xr3:uid="{3C6E783B-60EC-F249-9BBB-E5313DD53FB2}" name="population" dataDxfId="36">
       <calculatedColumnFormula array="1">Table41520[population]-(Table51621[[#This Row],[infections]]+Table51621[[#This Row],[deaths]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -24847,15 +24806,15 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{FC954438-C961-AE4A-A490-58381C034BF8}" name="Table61722" displayName="Table61722" ref="N8:P9" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{FC954438-C961-AE4A-A490-58381C034BF8}" name="Table61722" displayName="Table61722" ref="N8:P9" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{B7560F4C-52C8-E34B-AD0A-0C02AD7A6C08}" name="deaths" dataDxfId="23">
+    <tableColumn id="1" xr3:uid="{B7560F4C-52C8-E34B-AD0A-0C02AD7A6C08}" name="deaths" dataDxfId="33">
       <calculatedColumnFormula>Table31419[[#This Row],[projected deaths at 81% prevalence]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{24D708A2-8BA3-4744-8C40-D1EEBD44BE67}" name="infections" dataDxfId="22">
+    <tableColumn id="2" xr3:uid="{24D708A2-8BA3-4744-8C40-D1EEBD44BE67}" name="infections" dataDxfId="32">
       <calculatedColumnFormula>Table31419[[#This Row],[number of infections]]-Table31419[[#This Row],[projected deaths at 81% prevalence]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BAC9388F-C9DB-AC4D-A490-15460A77116A}" name="population" dataDxfId="21">
+    <tableColumn id="3" xr3:uid="{BAC9388F-C9DB-AC4D-A490-15460A77116A}" name="population" dataDxfId="31">
       <calculatedColumnFormula array="1">Table41520[population]-(O9+N9)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -24864,12 +24823,12 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{4863356E-2B9D-634F-956A-5CCE0DE37682}" name="Table2131823" displayName="Table2131823" ref="K4:L5" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{4863356E-2B9D-634F-956A-5CCE0DE37682}" name="Table2131823" displayName="Table2131823" ref="K4:L5" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <tableColumns count="2">
-    <tableColumn id="3" xr3:uid="{82EE0150-82AE-AB42-A252-FCDA50CCEC9C}" name="deaths" dataDxfId="18">
+    <tableColumn id="3" xr3:uid="{82EE0150-82AE-AB42-A252-FCDA50CCEC9C}" name="deaths" dataDxfId="28">
       <calculatedColumnFormula>data!B5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{A0224290-B752-E042-AF6E-6106E8DCF67B}" name="estimated number of infections" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{A0224290-B752-E042-AF6E-6106E8DCF67B}" name="estimated number of infections" dataDxfId="27">
       <calculatedColumnFormula>data!F5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -24878,12 +24837,12 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{0F9770C3-F64A-8642-8C75-69CA9E2B88BB}" name="Table3141924" displayName="Table3141924" ref="K8:L9" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{0F9770C3-F64A-8642-8C75-69CA9E2B88BB}" name="Table3141924" displayName="Table3141924" ref="K8:L9" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <tableColumns count="2">
-    <tableColumn id="3" xr3:uid="{38BDA4EE-AB4B-1B45-97FA-43E969A7AA8E}" name="projected deaths at 81% prevalence" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{38BDA4EE-AB4B-1B45-97FA-43E969A7AA8E}" name="projected deaths at 81% prevalence" dataDxfId="24">
       <calculatedColumnFormula>data!H5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{28263471-4CB5-FA42-BA4B-7E8E7E1BEAA5}" name="number of infections" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{28263471-4CB5-FA42-BA4B-7E8E7E1BEAA5}" name="number of infections" dataDxfId="23">
       <calculatedColumnFormula>data!G5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -24892,9 +24851,9 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{B19FBBC7-36CC-A844-A1C7-458ABE012AD6}" name="Table4152025" displayName="Table4152025" ref="K11:K12" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{B19FBBC7-36CC-A844-A1C7-458ABE012AD6}" name="Table4152025" displayName="Table4152025" ref="K11:K12" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{5514E89F-165C-9249-9681-75DACE02926B}" name="population" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{5514E89F-165C-9249-9681-75DACE02926B}" name="population" dataDxfId="20">
       <calculatedColumnFormula>data!C5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -24903,15 +24862,15 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{7F705DA8-B332-5D46-899A-589255D616B4}" name="Table5162126" displayName="Table5162126" ref="N4:P5" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{7F705DA8-B332-5D46-899A-589255D616B4}" name="Table5162126" displayName="Table5162126" ref="N4:P5" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FADB59F1-A516-2A46-BDC0-5B29FD45563E}" name="deaths" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{FADB59F1-A516-2A46-BDC0-5B29FD45563E}" name="deaths" dataDxfId="17">
       <calculatedColumnFormula>Table2131823[[#This Row],[deaths]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B86124CD-BF81-6248-B768-6164C47E35A6}" name="infections" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{B86124CD-BF81-6248-B768-6164C47E35A6}" name="infections" dataDxfId="16">
       <calculatedColumnFormula>Table2131823[[#This Row],[estimated number of infections]]-N5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{081F0396-2223-D44C-B7A6-778B6BB7A4D6}" name="population" dataDxfId="5">
+    <tableColumn id="3" xr3:uid="{081F0396-2223-D44C-B7A6-778B6BB7A4D6}" name="population" dataDxfId="15">
       <calculatedColumnFormula array="1">Table4152025[population]-(Table5162126[[#This Row],[infections]]+Table5162126[[#This Row],[deaths]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -24920,12 +24879,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A6CA9C6A-2531-2B4B-8FAF-58B7CE42D209}" name="Table3" displayName="Table3" ref="K8:L9" totalsRowShown="0" headerRowDxfId="77" dataDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A6CA9C6A-2531-2B4B-8FAF-58B7CE42D209}" name="Table3" displayName="Table3" ref="K8:L9" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
   <tableColumns count="2">
-    <tableColumn id="3" xr3:uid="{7D8A9872-A8DB-7E4F-85C7-887729C862CC}" name="projected deaths at 81% prevalence" dataDxfId="79">
+    <tableColumn id="3" xr3:uid="{7D8A9872-A8DB-7E4F-85C7-887729C862CC}" name="projected deaths at 81% prevalence" dataDxfId="87">
       <calculatedColumnFormula>data!H2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{3C5B7FFB-7FAE-CA4C-B052-88563B410A23}" name="number of infections" dataDxfId="84">
+    <tableColumn id="1" xr3:uid="{3C5B7FFB-7FAE-CA4C-B052-88563B410A23}" name="number of infections" dataDxfId="86">
       <calculatedColumnFormula>data!G2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -24934,15 +24893,15 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{4F98D2C0-C5E4-D94B-A6A8-E0F3FF1D80AF}" name="Table6172227" displayName="Table6172227" ref="N8:P9" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{4F98D2C0-C5E4-D94B-A6A8-E0F3FF1D80AF}" name="Table6172227" displayName="Table6172227" ref="N8:P9" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9C469E6E-EC80-294D-B92A-3DC5B6C571FE}" name="deaths" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{9C469E6E-EC80-294D-B92A-3DC5B6C571FE}" name="deaths" dataDxfId="12">
       <calculatedColumnFormula>Table3141924[[#This Row],[projected deaths at 81% prevalence]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{DD82B430-41C2-2643-9826-EFEE811F580E}" name="infections" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{DD82B430-41C2-2643-9826-EFEE811F580E}" name="infections" dataDxfId="11">
       <calculatedColumnFormula>Table3141924[[#This Row],[number of infections]]-Table3141924[[#This Row],[projected deaths at 81% prevalence]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5F4E84A5-0BE1-244E-AD31-2A639034598D}" name="population" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{5F4E84A5-0BE1-244E-AD31-2A639034598D}" name="population" dataDxfId="10">
       <calculatedColumnFormula array="1">Table4152025[population]-(O9+N9)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -24951,21 +24910,21 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{06D03A02-55D4-514F-80A7-E6766F836180}" name="Table1" displayName="Table1" ref="A1:H5" totalsRowShown="0" headerRowDxfId="76" dataDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{06D03A02-55D4-514F-80A7-E6766F836180}" name="Table1" displayName="Table1" ref="A1:H5" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:H5" xr:uid="{CFC51504-B2BD-0348-AF40-9E28EEFE0406}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{83D2458A-BBAC-254F-9784-7E4CF229585E}" name="area" dataDxfId="92"/>
-    <tableColumn id="6" xr3:uid="{78E323B4-589E-BF43-B290-DA5DB82962E5}" name="deaths" dataDxfId="89"/>
-    <tableColumn id="2" xr3:uid="{0FEA8723-478D-D64A-AA53-906CC15B70E5}" name="population" dataDxfId="91"/>
-    <tableColumn id="5" xr3:uid="{ACA4CF98-00AC-ED44-AF5A-96D4FC80A888}" name="cases" dataDxfId="90"/>
-    <tableColumn id="7" xr3:uid="{F39933B7-21F9-A545-8552-480AF4911D1C}" name="prevalence" dataDxfId="88"/>
-    <tableColumn id="9" xr3:uid="{4D44F59A-FD3E-D94A-913B-0E2C3B6CC7E6}" name="estimated number of infections" dataDxfId="86">
+    <tableColumn id="1" xr3:uid="{83D2458A-BBAC-254F-9784-7E4CF229585E}" name="area" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{78E323B4-589E-BF43-B290-DA5DB82962E5}" name="deaths" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{0FEA8723-478D-D64A-AA53-906CC15B70E5}" name="population" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{ACA4CF98-00AC-ED44-AF5A-96D4FC80A888}" name="cases" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{F39933B7-21F9-A545-8552-480AF4911D1C}" name="prevalence" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{4D44F59A-FD3E-D94A-913B-0E2C3B6CC7E6}" name="estimated number of infections" dataDxfId="2">
       <calculatedColumnFormula>Table1[[#This Row],[population]]*Table1[[#This Row],[prevalence]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{B6D84FAD-9695-BC4F-8D7F-0E1F18FFDFDA}" name="number of infections at 81% prevalence" dataDxfId="85">
+    <tableColumn id="10" xr3:uid="{B6D84FAD-9695-BC4F-8D7F-0E1F18FFDFDA}" name="number of infections at 81% prevalence" dataDxfId="1">
       <calculatedColumnFormula>Table1[[#This Row],[population]]*0.81</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{52C792E5-13CC-D646-B591-5280A7562CF3}" name="projected deaths at 81% prevalence" dataDxfId="87">
+    <tableColumn id="3" xr3:uid="{52C792E5-13CC-D646-B591-5280A7562CF3}" name="projected deaths at 81% prevalence" dataDxfId="0">
       <calculatedColumnFormula>Table1[[#This Row],[deaths]]*0.81/Table1[[#This Row],[prevalence]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -24974,9 +24933,9 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3C0D7983-4F7F-554D-8761-730075E27FCA}" name="Table4" displayName="Table4" ref="K11:K12" totalsRowShown="0" headerRowDxfId="73" dataDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3C0D7983-4F7F-554D-8761-730075E27FCA}" name="Table4" displayName="Table4" ref="K11:K12" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{4FC70CE1-3458-4641-B584-0FBA0119753C}" name="population" dataDxfId="75">
+    <tableColumn id="1" xr3:uid="{4FC70CE1-3458-4641-B584-0FBA0119753C}" name="population" dataDxfId="83">
       <calculatedColumnFormula>data!C2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -24985,15 +24944,15 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E8A37B68-5552-5C4A-8F96-91516F4E7A10}" name="Table5" displayName="Table5" ref="N4:P5" totalsRowShown="0" headerRowDxfId="64" dataDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E8A37B68-5552-5C4A-8F96-91516F4E7A10}" name="Table5" displayName="Table5" ref="N4:P5" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{60CA5D12-B956-D342-82EB-BD808A3A3601}" name="deaths" dataDxfId="72">
+    <tableColumn id="1" xr3:uid="{60CA5D12-B956-D342-82EB-BD808A3A3601}" name="deaths" dataDxfId="80">
       <calculatedColumnFormula>Table2[[#This Row],[deaths]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{7BFC9353-E4A2-3143-AA65-686B731F3A20}" name="infections" dataDxfId="71">
+    <tableColumn id="2" xr3:uid="{7BFC9353-E4A2-3143-AA65-686B731F3A20}" name="infections" dataDxfId="79">
       <calculatedColumnFormula>Table2[[#This Row],[estimated number of infections]]-N5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BCB75EDD-97D2-B44F-AFB2-ECEB5A52DA81}" name="population" dataDxfId="70">
+    <tableColumn id="3" xr3:uid="{BCB75EDD-97D2-B44F-AFB2-ECEB5A52DA81}" name="population" dataDxfId="78">
       <calculatedColumnFormula array="1">Table4[population]-(Table5[[#This Row],[infections]]+Table5[[#This Row],[deaths]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -25002,15 +24961,15 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D761ABC3-3D7E-5F46-B26D-BB4379107720}" name="Table6" displayName="Table6" ref="N8:P9" totalsRowShown="0" headerRowDxfId="63" dataDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D761ABC3-3D7E-5F46-B26D-BB4379107720}" name="Table6" displayName="Table6" ref="N8:P9" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A7AFD05D-7BC4-B04C-B1C1-1D7136959CD8}" name="deaths" dataDxfId="68">
+    <tableColumn id="1" xr3:uid="{A7AFD05D-7BC4-B04C-B1C1-1D7136959CD8}" name="deaths" dataDxfId="75">
       <calculatedColumnFormula>Table3[[#This Row],[projected deaths at 81% prevalence]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D924AA7E-2CC7-4D43-8D6B-BFBA1E2F2176}" name="infections" dataDxfId="67">
+    <tableColumn id="2" xr3:uid="{D924AA7E-2CC7-4D43-8D6B-BFBA1E2F2176}" name="infections" dataDxfId="74">
       <calculatedColumnFormula>Table3[[#This Row],[number of infections]]-Table3[[#This Row],[projected deaths at 81% prevalence]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0E93C2E3-97A4-5F43-8722-C4A83FC2585B}" name="population" dataDxfId="66">
+    <tableColumn id="3" xr3:uid="{0E93C2E3-97A4-5F43-8722-C4A83FC2585B}" name="population" dataDxfId="73">
       <calculatedColumnFormula array="1">Table4[population]-(O9+N9)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -25019,12 +24978,12 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{56DA9B4D-517A-C145-9BC1-62CF94988E47}" name="Table213" displayName="Table213" ref="K4:L5" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{56DA9B4D-517A-C145-9BC1-62CF94988E47}" name="Table213" displayName="Table213" ref="K4:L5" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
   <tableColumns count="2">
-    <tableColumn id="3" xr3:uid="{D6448E5D-51F6-B644-816D-3C13B20046E6}" name="deaths" dataDxfId="60">
+    <tableColumn id="3" xr3:uid="{D6448E5D-51F6-B644-816D-3C13B20046E6}" name="deaths" dataDxfId="70">
       <calculatedColumnFormula>data!B3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{2AF07C21-1EC8-4F47-951F-FDBB73154890}" name="estimated number of infections" dataDxfId="59">
+    <tableColumn id="1" xr3:uid="{2AF07C21-1EC8-4F47-951F-FDBB73154890}" name="estimated number of infections" dataDxfId="69">
       <calculatedColumnFormula>data!F3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -25033,12 +24992,12 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{39A1EB80-EAF8-F246-A4FF-094E04AB3C0A}" name="Table314" displayName="Table314" ref="K8:L9" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{39A1EB80-EAF8-F246-A4FF-094E04AB3C0A}" name="Table314" displayName="Table314" ref="K8:L9" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
   <tableColumns count="2">
-    <tableColumn id="3" xr3:uid="{79893942-9BB0-E349-8D6E-328CFD81E53D}" name="projected deaths at 81% prevalence" dataDxfId="56">
+    <tableColumn id="3" xr3:uid="{79893942-9BB0-E349-8D6E-328CFD81E53D}" name="projected deaths at 81% prevalence" dataDxfId="66">
       <calculatedColumnFormula>data!H3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{253A7139-E89E-7743-BA78-E3A1D80D64CC}" name="number of infections" dataDxfId="55">
+    <tableColumn id="1" xr3:uid="{253A7139-E89E-7743-BA78-E3A1D80D64CC}" name="number of infections" dataDxfId="65">
       <calculatedColumnFormula>data!G3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -25047,9 +25006,9 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{500F593C-3038-CA49-AC98-0BBA694BE38D}" name="Table415" displayName="Table415" ref="K11:K12" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{500F593C-3038-CA49-AC98-0BBA694BE38D}" name="Table415" displayName="Table415" ref="K11:K12" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{2C1D4FA2-690F-734D-876C-272740594F2E}" name="population" dataDxfId="52">
+    <tableColumn id="1" xr3:uid="{2C1D4FA2-690F-734D-876C-272740594F2E}" name="population" dataDxfId="62">
       <calculatedColumnFormula>data!C3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -25058,15 +25017,15 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{B9BBB74E-E8CC-104C-8D29-987D39B5B0B9}" name="Table516" displayName="Table516" ref="N4:P5" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{B9BBB74E-E8CC-104C-8D29-987D39B5B0B9}" name="Table516" displayName="Table516" ref="N4:P5" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{23DC4DE4-93DB-5A49-8613-2282BE919F57}" name="deaths" dataDxfId="49">
+    <tableColumn id="1" xr3:uid="{23DC4DE4-93DB-5A49-8613-2282BE919F57}" name="deaths" dataDxfId="59">
       <calculatedColumnFormula>Table213[[#This Row],[deaths]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{FEE56615-8DF2-CE4D-A85D-051908B22A75}" name="infections" dataDxfId="48">
+    <tableColumn id="2" xr3:uid="{FEE56615-8DF2-CE4D-A85D-051908B22A75}" name="infections" dataDxfId="58">
       <calculatedColumnFormula>Table213[[#This Row],[estimated number of infections]]-N5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0B07E1D7-5C80-7340-AF25-61083F962D20}" name="population" dataDxfId="47">
+    <tableColumn id="3" xr3:uid="{0B07E1D7-5C80-7340-AF25-61083F962D20}" name="population" dataDxfId="57">
       <calculatedColumnFormula array="1">Table415[population]-(Table516[[#This Row],[infections]]+Table516[[#This Row],[deaths]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -25373,8 +25332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F2722A-BA5A-8646-9F79-9A5DAC7DF673}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -25696,9 +25655,6 @@
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
       <c r="I18" s="18"/>
-      <c r="K18" s="2" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="16"/>

</xml_diff>